<commit_message>
Added tests and made minor changes
</commit_message>
<xml_diff>
--- a/documentation/H17_S17_Basic_Strategy.xlsx
+++ b/documentation/H17_S17_Basic_Strategy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpqui\Documents\Projects\Blackjack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpqui\Documents\Projects\blackjack\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,6 @@
     <sheet name="4-8 Decks, Hit Soft 17" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="17">
   <si>
     <t>J</t>
   </si>
@@ -145,6 +144,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -154,17 +159,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -232,174 +231,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -693,11 +524,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J14" sqref="J14"/>
+      <selection pane="topRight" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -706,27 +537,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A2" s="7"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="3">
         <v>2</v>
       </c>
@@ -1624,27 +1455,27 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A24" s="8"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="3">
         <v>2</v>
       </c>
@@ -1686,46 +1517,46 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A25" s="10">
+      <c r="A25" s="7">
         <v>12</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="N25" s="9" t="s">
+      <c r="B25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2132,27 +1963,27 @@
       <c r="A36" s="4"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A38" s="8"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="3">
         <v>2</v>
       </c>
@@ -2591,177 +2422,45 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A49" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A50" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A51" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N51" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2774,7 +2473,7 @@
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:N37"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:N20 B26:N34 B39:N51">
+  <conditionalFormatting sqref="B3:N20 B26:N34 B39:N48">
     <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"S"</formula>
     </cfRule>
@@ -2787,7 +2486,7 @@
       <formula>"Ds"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39:N51">
+  <conditionalFormatting sqref="B39:N48">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Ph"</formula>
     </cfRule>
@@ -2795,7 +2494,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:N34 B39:N51 B3:N20">
+  <conditionalFormatting sqref="B25:N34 B3:N20 B39:N48">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"H"</formula>
     </cfRule>
@@ -2807,11 +2506,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I14" sqref="I14"/>
+      <selection pane="topRight" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2820,27 +2519,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" s="8"/>
+      <c r="A2" s="10"/>
       <c r="B2" s="3">
         <v>2</v>
       </c>
@@ -3674,27 +3373,27 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A24" s="8"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="3">
         <v>2</v>
       </c>
@@ -3736,46 +3435,46 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A25" s="10">
+      <c r="A25" s="7">
         <v>12</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="N25" s="9" t="s">
+      <c r="B25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4176,27 +3875,27 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A38" s="8"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="3">
         <v>2</v>
       </c>
@@ -4635,177 +4334,45 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A49" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A50" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A51" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N51" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4818,7 +4385,7 @@
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:N37"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:N20 B26:N34 B39:N51">
+  <conditionalFormatting sqref="B3:N20 B26:N34 B39:N48">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Dh"</formula>
     </cfRule>
@@ -4831,7 +4398,7 @@
       <formula>"Ds"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39:N51">
+  <conditionalFormatting sqref="B39:N48">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Ph"</formula>
     </cfRule>
@@ -4839,7 +4406,7 @@
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:N34 B39:N51 B3:N20">
+  <conditionalFormatting sqref="B25:N34 B3:N20 B39:N48">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"H"</formula>
     </cfRule>

</xml_diff>